<commit_message>
cleanup | indic bn calculated
</commit_message>
<xml_diff>
--- a/testRun1__rouge/rouge_scores.xlsx
+++ b/testRun1__rouge/rouge_scores.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\Score\testRun1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\Score\testRun1__rouge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418DA198-4572-4DFA-AF96-E2D2DC3190B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB01177D-A3C2-4FB1-BE84-29DCD2D8CF5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
+  <si>
+    <t>Generated-Bangla-1-Shot</t>
+  </si>
+  <si>
+    <t>Generated-Bangla-10-Shot</t>
+  </si>
+  <si>
+    <t>Generated-Bangla-25-Shot</t>
+  </si>
+  <si>
+    <t>bnbphoneticparser</t>
+  </si>
+  <si>
+    <t>Google Translate</t>
+  </si>
+  <si>
+    <t>Indic Transliteration</t>
+  </si>
   <si>
     <t>rouge-1</t>
   </si>
@@ -40,26 +58,14 @@
     <t>f</t>
   </si>
   <si>
-    <t>Generated-Bangla-1-Shot</t>
-  </si>
-  <si>
-    <t>Generated-Bangla-10-Shot</t>
-  </si>
-  <si>
-    <t>Generated-Bangla-25-Shot</t>
-  </si>
-  <si>
-    <t>bnbphoneticparser</t>
-  </si>
-  <si>
-    <t>Google Translate</t>
+    <t>BN Transliterate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +86,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -89,7 +105,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -121,20 +137,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,245 +490,330 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="15" width="9.140625" style="2"/>
+    <col min="1" max="15" width="9.140625" style="2" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="2"/>
+    <col min="17" max="18" width="9.140625" style="2" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4" t="s">
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4" t="s">
+      <c r="B3">
+        <v>0.43984369381788302</v>
+      </c>
+      <c r="C3">
+        <v>0.22908146525876699</v>
+      </c>
+      <c r="D3">
+        <v>0.43760396538821011</v>
+      </c>
+      <c r="E3">
+        <v>0.500479254154929</v>
+      </c>
+      <c r="F3">
+        <v>0.28719892991879298</v>
+      </c>
+      <c r="G3">
+        <v>0.49907346422227999</v>
+      </c>
+      <c r="H3">
+        <v>0.51869765931721401</v>
+      </c>
+      <c r="I3">
+        <v>0.31266382010522897</v>
+      </c>
+      <c r="J3">
+        <v>0.51694390435503701</v>
+      </c>
+      <c r="K3">
+        <v>0.31880124124463399</v>
+      </c>
+      <c r="L3">
+        <v>0.11538107782900001</v>
+      </c>
+      <c r="M3">
+        <v>0.31846778945399101</v>
+      </c>
+      <c r="N3">
+        <v>0.55806875911473108</v>
+      </c>
+      <c r="O3">
+        <v>0.35238216778344811</v>
+      </c>
+      <c r="P3">
+        <v>0.55741871665178999</v>
+      </c>
+      <c r="Q3">
+        <v>5.7492306237474013E-2</v>
+      </c>
+      <c r="R3">
+        <v>6.9781830413290008E-3</v>
+      </c>
+      <c r="S3">
+        <v>5.7415917879060002E-2</v>
+      </c>
+      <c r="T3">
+        <v>0.41015464410297298</v>
+      </c>
+      <c r="U3">
+        <v>0.18284690881499299</v>
+      </c>
+      <c r="V3">
+        <v>0.40979640516917498</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
+      <c r="B4">
+        <v>0.45977261105917311</v>
+      </c>
+      <c r="C4">
+        <v>0.240502401067689</v>
+      </c>
+      <c r="D4">
+        <v>0.45738653580815197</v>
+      </c>
+      <c r="E4">
+        <v>0.51320192095704709</v>
+      </c>
+      <c r="F4">
+        <v>0.29514958875731401</v>
+      </c>
+      <c r="G4">
+        <v>0.51158715415301703</v>
+      </c>
+      <c r="H4">
+        <v>0.54294880126850509</v>
+      </c>
+      <c r="I4">
+        <v>0.32849601207100998</v>
+      </c>
+      <c r="J4">
+        <v>0.54102058080751403</v>
+      </c>
+      <c r="K4">
+        <v>0.32385995214934798</v>
+      </c>
+      <c r="L4">
+        <v>0.116424078822172</v>
+      </c>
+      <c r="M4">
+        <v>0.32352086058880603</v>
+      </c>
+      <c r="N4">
+        <v>0.56577547545870299</v>
+      </c>
+      <c r="O4">
+        <v>0.357906588815182</v>
+      </c>
+      <c r="P4">
+        <v>0.56513734827638507</v>
+      </c>
+      <c r="Q4">
+        <v>5.8741533672161013E-2</v>
+      </c>
+      <c r="R4">
+        <v>7.0762004077630008E-3</v>
+      </c>
+      <c r="S4">
+        <v>5.8665145313747002E-2</v>
+      </c>
+      <c r="T4">
+        <v>0.41862849364864302</v>
+      </c>
+      <c r="U4">
+        <v>0.18697854486277499</v>
+      </c>
+      <c r="V4">
+        <v>0.41834709776586798</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.43984369381788302</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0.22908146525876699</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.43760396538821011</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.500479254154929</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.28719892991879298</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0.49907346422227999</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0.51869765931721401</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0.31266382010522897</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0.51694390435503701</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0.31880124124463399</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0.11538107782900001</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0.31846778945399101</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0.55806875911473108</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0.35238216778344811</v>
-      </c>
-      <c r="P3" s="2">
-        <v>0.55741871665178999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.45977261105917311</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.240502401067689</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.45738653580815197</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.51320192095704709</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.29514958875731401</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0.51158715415301703</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0.54294880126850509</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0.32849601207100998</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0.54102058080751403</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0.32385995214934798</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0.116424078822172</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0.32352086058880603</v>
-      </c>
-      <c r="N4" s="2">
-        <v>0.56577547545870299</v>
-      </c>
-      <c r="O4" s="2">
-        <v>0.357906588815182</v>
-      </c>
-      <c r="P4" s="2">
-        <v>0.56513734827638507</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
+        <v>11</v>
+      </c>
+      <c r="B5">
         <v>0.44565180541235699</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>0.23237642307395401</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>0.44337007070620499</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>0.50160696454103804</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5">
         <v>0.28731565013791599</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>0.50018564037552704</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5">
         <v>0.52598519660783705</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5">
         <v>0.31738185098353</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5">
         <v>0.52418809368705599</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5">
         <v>0.31922296763642699</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5">
         <v>0.115095341184072</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5">
         <v>0.31888680439355199</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5">
         <v>0.55909801522082703</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5">
         <v>0.35304281121876802</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5">
         <v>0.55845727627955799</v>
+      </c>
+      <c r="Q5">
+        <v>5.7615692146219998E-2</v>
+      </c>
+      <c r="R5">
+        <v>7.0008923221419996E-3</v>
+      </c>
+      <c r="S5">
+        <v>5.7539303787806008E-2</v>
+      </c>
+      <c r="T5">
+        <v>0.41241320920678698</v>
+      </c>
+      <c r="U5">
+        <v>0.18370433699149299</v>
+      </c>
+      <c r="V5">
+        <v>0.41209968915547202</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>

</xml_diff>

<commit_message>
G Input Tools Score calculated
</commit_message>
<xml_diff>
--- a/testRun1__rouge/rouge_scores.xlsx
+++ b/testRun1__rouge/rouge_scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\Score\testRun1__rouge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB01177D-A3C2-4FB1-BE84-29DCD2D8CF5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98280F7D-6B5A-4191-993B-696DE94A88F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
   <si>
     <t>Generated-Bangla-1-Shot</t>
   </si>
@@ -40,6 +40,9 @@
     <t>Indic Transliteration</t>
   </si>
   <si>
+    <t>BN Transliterate</t>
+  </si>
+  <si>
     <t>rouge-1</t>
   </si>
   <si>
@@ -58,14 +61,14 @@
     <t>f</t>
   </si>
   <si>
-    <t>BN Transliterate</t>
+    <t>G Input Tools</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +99,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -105,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -167,11 +175,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -182,6 +205,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -490,125 +516,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="15" width="9.140625" style="2" customWidth="1"/>
     <col min="16" max="16" width="12.7109375" style="2" customWidth="1"/>
-    <col min="17" max="18" width="9.140625" style="2" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="2"/>
+    <col min="17" max="19" width="9.140625" style="2" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="6" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="6" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="6" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="6" t="s">
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="6" t="s">
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="U2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="T2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="U2" s="5" t="s">
+      <c r="V2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="W2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="X2" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="Y2" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>0.43984369381788302</v>
@@ -673,10 +713,19 @@
       <c r="V3">
         <v>0.40979640516917498</v>
       </c>
+      <c r="W3">
+        <v>0.55684117684763001</v>
+      </c>
+      <c r="X3">
+        <v>0.33718831327595</v>
+      </c>
+      <c r="Y3">
+        <v>0.55627164361152504</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>0.45977261105917311</v>
@@ -741,10 +790,19 @@
       <c r="V4">
         <v>0.41834709776586798</v>
       </c>
+      <c r="W4">
+        <v>0.56729346076986309</v>
+      </c>
+      <c r="X4">
+        <v>0.34347278014420002</v>
+      </c>
+      <c r="Y4">
+        <v>0.56676969700248803</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>0.44565180541235699</v>
@@ -809,9 +867,19 @@
       <c r="V5">
         <v>0.41209968915547202</v>
       </c>
+      <c r="W5">
+        <v>0.55863058570274704</v>
+      </c>
+      <c r="X5">
+        <v>0.33789264200228097</v>
+      </c>
+      <c r="Y5">
+        <v>0.55808714058408604</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="W1:Y1"/>
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>

</xml_diff>